<commit_message>
Supported Auto random play after 3 min
</commit_message>
<xml_diff>
--- a/ICON16x16.xlsx
+++ b/ICON16x16.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Data\work\Sipeed_Longan_Nano_Projects\gd32v_i2s_dac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BAFC4D-B939-434F-BE7C-F5B2C9A30426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E7CE07-08CC-4875-BED2-928CAD87FE20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="345" windowWidth="25110" windowHeight="15255" xr2:uid="{7E682170-0FA3-4D33-A3CA-4458C6F2D2D4}"/>
+    <workbookView xWindow="450" yWindow="225" windowWidth="28350" windowHeight="15255" xr2:uid="{7E682170-0FA3-4D33-A3CA-4458C6F2D2D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -515,7 +515,7 @@
   <dimension ref="J12:AI135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="AH9" sqref="AH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -547,7 +547,7 @@
       </c>
       <c r="AI12" t="str">
         <f>"0x"&amp;AE12&amp;",0x"&amp;AF12&amp;",0x"&amp;AE13&amp;",0x"&amp;AF13&amp;",0x"&amp;AE14&amp;",0x"&amp;AF14&amp;",0x"&amp;AE15&amp;",0x"&amp;AF15&amp;",0x"&amp;AE16&amp;",0x"&amp;AF16&amp;",0x"&amp;AE17&amp;",0x"&amp;AF17&amp;",0x"&amp;AE18&amp;",0x"&amp;AF18&amp;",0x"&amp;AE19&amp;",0x"&amp;AF19</f>
-        <v>0x00,0x00,0x80,0x00,0x80,0x01,0x80,0x07,0x80,0x0F,0x80,0x1F,0x80,0x18,0x80,0x10</v>
+        <v>0x00,0x00,0x80,0x00,0x80,0x01,0x80,0x07,0x80,0x0F,0x80,0x1E,0x80,0x18,0x80,0x10</v>
       </c>
     </row>
     <row r="13" spans="10:35" x14ac:dyDescent="0.4">
@@ -565,6 +565,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
+      <c r="W13" s="1"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="6"/>
       <c r="AE13" t="str">
@@ -691,9 +692,7 @@
       <c r="Q17" s="10">
         <v>1</v>
       </c>
-      <c r="R17" s="10">
-        <v>1</v>
-      </c>
+      <c r="R17" s="1"/>
       <c r="S17" s="10">
         <v>1</v>
       </c>
@@ -715,7 +714,7 @@
       </c>
       <c r="AF17" t="str">
         <f t="shared" si="1"/>
-        <v>1F</v>
+        <v>1E</v>
       </c>
     </row>
     <row r="18" spans="10:35" x14ac:dyDescent="0.4">

</xml_diff>